<commit_message>
End worktime 13/10/2017, done view timekeepers
</commit_message>
<xml_diff>
--- a/files/timekeepers_import.xlsx
+++ b/files/timekeepers_import.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
@@ -14,7 +14,7 @@
   <externalReferences>
     <externalReference r:id="rId4"/>
   </externalReferences>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
@@ -24,7 +24,7 @@
     <author>Author</author>
   </authors>
   <commentList>
-    <comment ref="N18" authorId="0" shapeId="0">
+    <comment ref="N18" authorId="0">
       <text>
         <r>
           <rPr>
@@ -54,7 +54,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="33">
   <si>
     <t xml:space="preserve">CÔNG TY CỔ PHẦN CƠ ĐIỆN </t>
   </si>
@@ -155,19 +155,16 @@
   </si>
   <si>
     <t>Tan</t>
-  </si>
-  <si>
-    <t>CT</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="9">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -527,19 +524,11 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
     <sheetNames>
       <sheetName val="StartUp"/>
@@ -642,7 +631,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -674,10 +663,9 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -709,7 +697,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -885,14 +872,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:AT46"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="N10" sqref="N10"/>
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="AE9" sqref="AE9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="12"/>
   <cols>
     <col min="1" max="1" width="3.85546875" style="1" customWidth="1"/>
     <col min="2" max="2" width="18.85546875" style="18" customWidth="1"/>
@@ -940,13 +927,13 @@
     <col min="51" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:46">
       <c r="A1" s="19" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="22"/>
     </row>
-    <row r="2" spans="1:46" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:46" ht="15.75">
       <c r="A2" s="35" t="s">
         <v>1</v>
       </c>
@@ -996,7 +983,7 @@
       <c r="AQ2" s="42"/>
       <c r="AR2" s="42"/>
     </row>
-    <row r="3" spans="1:46" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:46" ht="15.75">
       <c r="B3" s="2"/>
       <c r="D3" s="20"/>
       <c r="E3" s="20"/>
@@ -1040,7 +1027,7 @@
       <c r="AQ3" s="20"/>
       <c r="AR3" s="20"/>
     </row>
-    <row r="4" spans="1:46" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:46" ht="12" customHeight="1">
       <c r="B4" s="2"/>
       <c r="D4" s="43" t="s">
         <v>23</v>
@@ -1088,7 +1075,7 @@
       <c r="AS4" s="43"/>
       <c r="AT4" s="43"/>
     </row>
-    <row r="5" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:46">
       <c r="A5" s="34" t="s">
         <v>2</v>
       </c>
@@ -1154,7 +1141,7 @@
       <c r="AS5" s="34"/>
       <c r="AT5" s="34"/>
     </row>
-    <row r="6" spans="1:46" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:46" s="2" customFormat="1">
       <c r="A6" s="34"/>
       <c r="B6" s="36"/>
       <c r="C6" s="38"/>
@@ -1280,7 +1267,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="7" spans="1:46" s="25" customFormat="1" ht="12.75" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:46" s="25" customFormat="1" ht="12.75">
       <c r="A7" s="5">
         <v>1</v>
       </c>
@@ -1294,23 +1281,23 @@
         <v>4</v>
       </c>
       <c r="E7" s="7"/>
-      <c r="F7" s="6" t="s">
+      <c r="F7" s="6">
         <v>8</v>
       </c>
       <c r="G7" s="6">
         <v>8</v>
       </c>
-      <c r="H7" s="6" t="s">
-        <v>33</v>
+      <c r="H7" s="6">
+        <v>8</v>
       </c>
       <c r="I7" s="6">
         <v>8</v>
       </c>
-      <c r="J7" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="K7" s="6" t="s">
-        <v>33</v>
+      <c r="J7" s="6">
+        <v>8</v>
+      </c>
+      <c r="K7" s="6">
+        <v>8</v>
       </c>
       <c r="L7" s="7"/>
       <c r="M7" s="6">
@@ -1375,11 +1362,11 @@
       </c>
       <c r="AI7" s="8">
         <f>SUM(D7:AH7)/8+ COUNTIF(D8:AH8,"CT")</f>
-        <v>21.5</v>
+        <v>25.5</v>
       </c>
       <c r="AJ7" s="5">
         <f>AG8+Z8+S8+L8+E8</f>
-        <v>24</v>
+        <v>16</v>
       </c>
       <c r="AK7" s="5">
         <f>SUM(D8:AH8)-AJ7</f>
@@ -1395,7 +1382,7 @@
       </c>
       <c r="AN7" s="5">
         <f>COUNTIF(D7:AH7,"Ro")</f>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="AO7" s="5">
         <f>COUNTIF(D7:AH7,"R")</f>
@@ -1416,7 +1403,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:46" s="30" customFormat="1" ht="12.75" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:46" s="30" customFormat="1" ht="12.75">
       <c r="A8" s="9"/>
       <c r="B8" s="31"/>
       <c r="C8" s="32"/>
@@ -1471,9 +1458,7 @@
       </c>
       <c r="AE8" s="12"/>
       <c r="AF8" s="14"/>
-      <c r="AG8" s="13">
-        <v>8</v>
-      </c>
+      <c r="AG8" s="13"/>
       <c r="AH8" s="12"/>
       <c r="AI8" s="15"/>
       <c r="AJ8" s="9"/>
@@ -1488,7 +1473,7 @@
       <c r="AS8" s="9"/>
       <c r="AT8" s="9"/>
     </row>
-    <row r="9" spans="1:46" s="25" customFormat="1" ht="12.75" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:46" s="25" customFormat="1" ht="12.75">
       <c r="A9" s="5">
         <v>2</v>
       </c>
@@ -1624,7 +1609,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:46" s="25" customFormat="1" ht="12.75" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:46" s="25" customFormat="1" ht="12.75">
       <c r="A10" s="12"/>
       <c r="B10" s="26"/>
       <c r="C10" s="12"/>
@@ -1672,7 +1657,7 @@
       <c r="AS10" s="12"/>
       <c r="AT10" s="12"/>
     </row>
-    <row r="11" spans="1:46" s="25" customFormat="1" ht="12.75" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:46" s="25" customFormat="1" ht="12.75">
       <c r="A11" s="5">
         <v>3</v>
       </c>
@@ -1808,7 +1793,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:46" s="25" customFormat="1" ht="12.75" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:46" s="25" customFormat="1" ht="12.75">
       <c r="A12" s="12"/>
       <c r="B12" s="26"/>
       <c r="C12" s="12"/>
@@ -1856,7 +1841,7 @@
       <c r="AS12" s="12"/>
       <c r="AT12" s="12"/>
     </row>
-    <row r="13" spans="1:46" s="25" customFormat="1" ht="12.75" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:46" s="25" customFormat="1" ht="12.75">
       <c r="A13" s="5"/>
       <c r="B13" s="24"/>
       <c r="C13" s="5"/>
@@ -1904,7 +1889,7 @@
       <c r="AS13" s="5"/>
       <c r="AT13" s="5"/>
     </row>
-    <row r="14" spans="1:46" s="25" customFormat="1" ht="12.75" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:46" s="25" customFormat="1" ht="12.75">
       <c r="A14" s="12"/>
       <c r="B14" s="26"/>
       <c r="C14" s="12"/>
@@ -1952,7 +1937,7 @@
       <c r="AS14" s="12"/>
       <c r="AT14" s="12"/>
     </row>
-    <row r="15" spans="1:46" s="25" customFormat="1" ht="12.75" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:46" s="25" customFormat="1" ht="12.75">
       <c r="A15" s="5"/>
       <c r="B15" s="24"/>
       <c r="C15" s="5"/>
@@ -2000,7 +1985,7 @@
       <c r="AS15" s="5"/>
       <c r="AT15" s="5"/>
     </row>
-    <row r="16" spans="1:46" s="25" customFormat="1" ht="12.75" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:46" s="25" customFormat="1" ht="12.75">
       <c r="A16" s="12"/>
       <c r="B16" s="26"/>
       <c r="C16" s="12"/>
@@ -2048,7 +2033,7 @@
       <c r="AS16" s="12"/>
       <c r="AT16" s="12"/>
     </row>
-    <row r="17" spans="1:46" s="25" customFormat="1" ht="12.75" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:46" s="25" customFormat="1" ht="12.75">
       <c r="A17" s="5"/>
       <c r="B17" s="24"/>
       <c r="C17" s="5"/>
@@ -2096,7 +2081,7 @@
       <c r="AS17" s="5"/>
       <c r="AT17" s="5"/>
     </row>
-    <row r="18" spans="1:46" s="25" customFormat="1" ht="12.75" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:46" s="25" customFormat="1" ht="12.75">
       <c r="A18" s="12"/>
       <c r="B18" s="26"/>
       <c r="C18" s="12"/>
@@ -2144,7 +2129,7 @@
       <c r="AS18" s="12"/>
       <c r="AT18" s="12"/>
     </row>
-    <row r="19" spans="1:46" s="25" customFormat="1" ht="12.75" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:46" s="25" customFormat="1" ht="12.75">
       <c r="A19" s="5"/>
       <c r="B19" s="24"/>
       <c r="C19" s="5"/>
@@ -2192,7 +2177,7 @@
       <c r="AS19" s="5"/>
       <c r="AT19" s="5"/>
     </row>
-    <row r="20" spans="1:46" s="25" customFormat="1" ht="12.75" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:46" s="25" customFormat="1" ht="12.75">
       <c r="A20" s="12"/>
       <c r="B20" s="26"/>
       <c r="C20" s="12"/>
@@ -2240,7 +2225,7 @@
       <c r="AS20" s="12"/>
       <c r="AT20" s="12"/>
     </row>
-    <row r="21" spans="1:46" s="25" customFormat="1" ht="12.75" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:46" s="25" customFormat="1" ht="12.75">
       <c r="A21" s="5"/>
       <c r="B21" s="24"/>
       <c r="C21" s="5"/>
@@ -2288,7 +2273,7 @@
       <c r="AS21" s="5"/>
       <c r="AT21" s="5"/>
     </row>
-    <row r="22" spans="1:46" s="25" customFormat="1" ht="12.75" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:46" s="25" customFormat="1" ht="12.75">
       <c r="A22" s="12"/>
       <c r="B22" s="26"/>
       <c r="C22" s="12"/>
@@ -2336,7 +2321,7 @@
       <c r="AS22" s="12"/>
       <c r="AT22" s="12"/>
     </row>
-    <row r="23" spans="1:46" s="25" customFormat="1" ht="12.75" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:46" s="25" customFormat="1" ht="12.75">
       <c r="A23" s="5"/>
       <c r="B23" s="24"/>
       <c r="C23" s="5"/>
@@ -2384,7 +2369,7 @@
       <c r="AS23" s="5"/>
       <c r="AT23" s="5"/>
     </row>
-    <row r="24" spans="1:46" s="25" customFormat="1" ht="12.75" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:46" s="25" customFormat="1" ht="12.75">
       <c r="A24" s="12"/>
       <c r="B24" s="26"/>
       <c r="C24" s="12"/>
@@ -2432,7 +2417,7 @@
       <c r="AS24" s="12"/>
       <c r="AT24" s="12"/>
     </row>
-    <row r="25" spans="1:46" s="25" customFormat="1" ht="12.75" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:46" s="25" customFormat="1" ht="12.75">
       <c r="A25" s="5"/>
       <c r="B25" s="24"/>
       <c r="C25" s="5"/>
@@ -2480,7 +2465,7 @@
       <c r="AS25" s="5"/>
       <c r="AT25" s="5"/>
     </row>
-    <row r="26" spans="1:46" s="25" customFormat="1" ht="12.75" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:46" s="25" customFormat="1" ht="12.75">
       <c r="A26" s="12"/>
       <c r="B26" s="26"/>
       <c r="C26" s="12"/>
@@ -2528,7 +2513,7 @@
       <c r="AS26" s="12"/>
       <c r="AT26" s="12"/>
     </row>
-    <row r="27" spans="1:46" s="25" customFormat="1" ht="12.75" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:46" s="25" customFormat="1" ht="12.75">
       <c r="A27" s="5"/>
       <c r="B27" s="24"/>
       <c r="C27" s="5"/>
@@ -2576,7 +2561,7 @@
       <c r="AS27" s="5"/>
       <c r="AT27" s="5"/>
     </row>
-    <row r="28" spans="1:46" s="25" customFormat="1" ht="12.75" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:46" s="25" customFormat="1" ht="12.75">
       <c r="A28" s="12"/>
       <c r="B28" s="26"/>
       <c r="C28" s="12"/>
@@ -2624,7 +2609,7 @@
       <c r="AS28" s="12"/>
       <c r="AT28" s="12"/>
     </row>
-    <row r="29" spans="1:46" s="25" customFormat="1" ht="12.75" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:46" s="25" customFormat="1" ht="12.75">
       <c r="A29" s="5"/>
       <c r="B29" s="24"/>
       <c r="C29" s="5"/>
@@ -2672,7 +2657,7 @@
       <c r="AS29" s="5"/>
       <c r="AT29" s="5"/>
     </row>
-    <row r="30" spans="1:46" s="25" customFormat="1" ht="12.75" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:46" s="25" customFormat="1" ht="12.75">
       <c r="A30" s="12"/>
       <c r="B30" s="26"/>
       <c r="C30" s="12"/>
@@ -2720,17 +2705,17 @@
       <c r="AS30" s="12"/>
       <c r="AT30" s="12"/>
     </row>
-    <row r="31" spans="1:46" s="27" customFormat="1" ht="12.75" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:46" s="27" customFormat="1" ht="12.75">
       <c r="B31" s="28"/>
       <c r="D31" s="29"/>
       <c r="E31" s="29"/>
       <c r="AI31" s="17">
         <f>SUM(AI7:AI30)</f>
-        <v>73</v>
+        <v>77</v>
       </c>
       <c r="AJ31" s="17">
         <f>SUM(AJ7:AJ30)</f>
-        <v>24</v>
+        <v>16</v>
       </c>
       <c r="AK31" s="17">
         <f>SUM(AK7:AK30)</f>
@@ -2741,12 +2726,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="2:42" x14ac:dyDescent="0.25">
+    <row r="33" spans="2:42">
       <c r="AK33" s="1" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="34" spans="2:42" x14ac:dyDescent="0.25">
+    <row r="34" spans="2:42">
       <c r="D34" s="1" t="s">
         <v>16</v>
       </c>
@@ -2757,7 +2742,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="35" spans="2:42" x14ac:dyDescent="0.25">
+    <row r="35" spans="2:42">
       <c r="H35" s="18" t="s">
         <v>19</v>
       </c>
@@ -2765,7 +2750,7 @@
       <c r="M35" s="2"/>
       <c r="T35" s="2"/>
     </row>
-    <row r="36" spans="2:42" x14ac:dyDescent="0.25">
+    <row r="36" spans="2:42">
       <c r="H36" s="18" t="s">
         <v>20</v>
       </c>
@@ -2780,7 +2765,7 @@
       <c r="AN36" s="19"/>
       <c r="AO36" s="19"/>
     </row>
-    <row r="37" spans="2:42" x14ac:dyDescent="0.25">
+    <row r="37" spans="2:42">
       <c r="H37" s="18" t="s">
         <v>21</v>
       </c>
@@ -2797,7 +2782,7 @@
       <c r="AO37" s="35"/>
       <c r="AP37" s="35"/>
     </row>
-    <row r="46" spans="2:42" x14ac:dyDescent="0.25">
+    <row r="46" spans="2:42">
       <c r="B46" s="18">
         <f>7300-630</f>
         <v>6670</v>
@@ -2825,24 +2810,24 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Backup before fix function import_xls timekeeper
</commit_message>
<xml_diff>
--- a/files/timekeepers_import.xlsx
+++ b/files/timekeepers_import.xlsx
@@ -15,12 +15,46 @@
     <externalReference r:id="rId4"/>
   </externalReferences>
   <calcPr calcId="124519"/>
-  <fileRecoveryPr repairLoad="1"/>
 </workbook>
 </file>
 
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <authors>
+    <author>Author</author>
+  </authors>
+  <commentList>
+    <comment ref="N18" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Author:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+ve 15 h 
+</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="33">
   <si>
     <t xml:space="preserve">CÔNG TY CỔ PHẦN CƠ ĐIỆN </t>
   </si>
@@ -130,7 +164,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
-  <fonts count="7">
+  <fonts count="9">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -168,6 +202,19 @@
       <sz val="9"/>
       <name val="Times New Roman"/>
       <family val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="6">
@@ -477,14 +524,6 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
 </styleSheet>
 </file>
 
@@ -837,7 +876,7 @@
   <dimension ref="A1:AT46"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4:AT4"/>
+      <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12"/>
@@ -847,8 +886,8 @@
     <col min="3" max="3" width="5.5703125" style="1" customWidth="1"/>
     <col min="4" max="4" width="3.42578125" style="1" customWidth="1"/>
     <col min="5" max="5" width="3" style="1" customWidth="1"/>
-    <col min="6" max="6" width="3.28515625" style="1" customWidth="1"/>
-    <col min="7" max="7" width="3" style="1" customWidth="1"/>
+    <col min="6" max="6" width="4" style="1" customWidth="1"/>
+    <col min="7" max="7" width="4.28515625" style="1" customWidth="1"/>
     <col min="8" max="8" width="3.28515625" style="1" customWidth="1"/>
     <col min="9" max="9" width="3.42578125" style="1" customWidth="1"/>
     <col min="10" max="10" width="3.140625" style="1" customWidth="1"/>
@@ -1239,30 +1278,30 @@
         <v>28</v>
       </c>
       <c r="D7" s="6">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="E7" s="7"/>
-      <c r="F7" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="G7" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="H7" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="I7" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="J7" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="K7" s="6" t="s">
-        <v>14</v>
+      <c r="F7" s="6">
+        <v>2.5</v>
+      </c>
+      <c r="G7" s="6">
+        <v>8</v>
+      </c>
+      <c r="H7" s="6">
+        <v>8</v>
+      </c>
+      <c r="I7" s="6">
+        <v>8</v>
+      </c>
+      <c r="J7" s="6">
+        <v>8</v>
+      </c>
+      <c r="K7" s="6">
+        <v>8</v>
       </c>
       <c r="L7" s="7"/>
       <c r="M7" s="6">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="N7" s="6">
         <v>8</v>
@@ -1323,15 +1362,15 @@
       </c>
       <c r="AI7" s="8">
         <f>SUM(D7:AH7)/8+ COUNTIF(D8:AH8,"CT")</f>
-        <v>19.5</v>
+        <v>24.8125</v>
       </c>
       <c r="AJ7" s="5">
         <f>AG8+Z8+S8+L8+E8</f>
-        <v>24</v>
+        <v>8</v>
       </c>
       <c r="AK7" s="5">
         <f>SUM(D8:AH8)-AJ7</f>
-        <v>12</v>
+        <v>2.5</v>
       </c>
       <c r="AL7" s="5">
         <f>D8/8</f>
@@ -1339,15 +1378,15 @@
       </c>
       <c r="AM7" s="5">
         <f>COUNTIF(D7:AG7,"P")</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AN7" s="5">
         <f>COUNTIF(D7:AH7,"Ro")</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AO7" s="5">
         <f>COUNTIF(D7:AH7,"R")</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AP7" s="5"/>
       <c r="AQ7" s="5">
@@ -1357,11 +1396,11 @@
       <c r="AR7" s="5"/>
       <c r="AS7" s="5">
         <f>COUNTIF(D7:AH7,"V")</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AT7" s="5">
         <f>COUNTIF(D7:AH7,"L")</f>
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="8" spans="1:46" s="30" customFormat="1" ht="12.75">
@@ -1372,20 +1411,18 @@
       <c r="E8" s="11">
         <v>8</v>
       </c>
-      <c r="F8" s="12"/>
-      <c r="G8" s="12"/>
+      <c r="F8" s="12">
+        <v>1</v>
+      </c>
+      <c r="G8" s="12">
+        <v>1.5</v>
+      </c>
       <c r="H8" s="12"/>
-      <c r="I8" s="12">
-        <v>2</v>
-      </c>
+      <c r="I8" s="12"/>
       <c r="J8" s="12"/>
       <c r="K8" s="12"/>
-      <c r="L8" s="13">
-        <v>8</v>
-      </c>
-      <c r="M8" s="12">
-        <v>2</v>
-      </c>
+      <c r="L8" s="13"/>
+      <c r="M8" s="12"/>
       <c r="N8" s="12"/>
       <c r="O8" s="12"/>
       <c r="P8" s="12"/>
@@ -1396,24 +1433,16 @@
       <c r="U8" s="12"/>
       <c r="V8" s="12"/>
       <c r="W8" s="12"/>
-      <c r="X8" s="12">
-        <v>2</v>
-      </c>
-      <c r="Y8" s="14">
-        <v>2</v>
-      </c>
+      <c r="X8" s="12"/>
+      <c r="Y8" s="14"/>
       <c r="Z8" s="13"/>
       <c r="AA8" s="12"/>
       <c r="AB8" s="12"/>
       <c r="AC8" s="12"/>
-      <c r="AD8" s="12">
-        <v>4</v>
-      </c>
+      <c r="AD8" s="12"/>
       <c r="AE8" s="12"/>
       <c r="AF8" s="14"/>
-      <c r="AG8" s="13">
-        <v>8</v>
-      </c>
+      <c r="AG8" s="13"/>
       <c r="AH8" s="12"/>
       <c r="AI8" s="15"/>
       <c r="AJ8" s="9"/>
@@ -1486,7 +1515,7 @@
       <c r="U9" s="6">
         <v>8</v>
       </c>
-      <c r="V9" s="6">
+      <c r="V9" s="12">
         <v>8</v>
       </c>
       <c r="W9" s="6">
@@ -2666,15 +2695,15 @@
       <c r="E31" s="29"/>
       <c r="AI31" s="17">
         <f>SUM(AI7:AI30)</f>
-        <v>71</v>
+        <v>76.3125</v>
       </c>
       <c r="AJ31" s="17">
         <f>SUM(AJ7:AJ30)</f>
-        <v>24</v>
+        <v>8</v>
       </c>
       <c r="AK31" s="17">
         <f>SUM(AK7:AK30)</f>
-        <v>12</v>
+        <v>2.5</v>
       </c>
       <c r="AL31" s="17">
         <f>SUM(AL7:AL30)</f>
@@ -2760,6 +2789,7 @@
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
 

</xml_diff>